<commit_message>
getting efficiency index correct. finalized on efficiency = Time/Strikes x probability(success). Probability of success = number of successful splits out of all cobble experiments. Plotted with boxplots (some with jitter). Nicely separates novices and experts. Although still some novices that overlap with experts. Might need to deal with more outliers. Need to fix original data sheet (clerical) errors.
</commit_message>
<xml_diff>
--- a/During experiment recording_fixed02.11.2014.xlsx
+++ b/During experiment recording_fixed02.11.2014.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="1920" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Bipolar" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2418" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2423" uniqueCount="260">
   <si>
     <t>Participant number</t>
   </si>
@@ -792,6 +792,15 @@
   </si>
   <si>
     <t>Split/No-split</t>
+  </si>
+  <si>
+    <t>Prob(success)</t>
+  </si>
+  <si>
+    <t>divided by 33</t>
+  </si>
+  <si>
+    <t>divided by 36</t>
   </si>
 </sst>
 </file>
@@ -855,8 +864,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="47">
+  <cellStyleXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -911,7 +928,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="47">
+  <cellStyles count="55">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -935,6 +952,10 @@
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -958,6 +979,10 @@
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6698,10 +6723,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H193"/>
+  <dimension ref="A1:J193"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView tabSelected="1" topLeftCell="A165" workbookViewId="0">
+      <selection activeCell="K192" sqref="K192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6712,7 +6737,7 @@
     <col min="5" max="5" width="11" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6737,8 +6762,14 @@
       <c r="H1" s="1" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="I1" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -6763,8 +6794,15 @@
       <c r="H2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="I2">
+        <f>14/33</f>
+        <v>0.42424242424242425</v>
+      </c>
+      <c r="J2" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -6789,8 +6827,12 @@
       <c r="H3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="I3">
+        <f>14/33</f>
+        <v>0.42424242424242425</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -6815,8 +6857,12 @@
       <c r="H4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="I4">
+        <f t="shared" ref="I4:I34" si="0">14/33</f>
+        <v>0.42424242424242425</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -6841,8 +6887,12 @@
       <c r="H5" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>0.42424242424242425</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -6867,8 +6917,12 @@
       <c r="H6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>0.42424242424242425</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -6893,8 +6947,12 @@
       <c r="H7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="I7">
+        <f t="shared" si="0"/>
+        <v>0.42424242424242425</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -6919,8 +6977,12 @@
       <c r="H8" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>0.42424242424242425</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -6945,8 +7007,12 @@
       <c r="H9" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>0.42424242424242425</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -6971,8 +7037,12 @@
       <c r="H10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>0.42424242424242425</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -6997,8 +7067,12 @@
       <c r="H11" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="I11">
+        <f t="shared" si="0"/>
+        <v>0.42424242424242425</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -7023,8 +7097,12 @@
       <c r="H12" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="I12">
+        <f t="shared" si="0"/>
+        <v>0.42424242424242425</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -7049,8 +7127,12 @@
       <c r="H13" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="1:8">
+      <c r="I13">
+        <f t="shared" si="0"/>
+        <v>0.42424242424242425</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -7075,8 +7157,12 @@
       <c r="H14" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="15" spans="1:8">
+      <c r="I14">
+        <f t="shared" si="0"/>
+        <v>0.42424242424242425</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -7101,8 +7187,12 @@
       <c r="H15" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="16" spans="1:8">
+      <c r="I15">
+        <f t="shared" si="0"/>
+        <v>0.42424242424242425</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -7127,8 +7217,12 @@
       <c r="H16" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="1:8">
+      <c r="I16">
+        <f t="shared" si="0"/>
+        <v>0.42424242424242425</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -7153,8 +7247,12 @@
       <c r="H17" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="18" spans="1:8">
+      <c r="I17">
+        <f t="shared" si="0"/>
+        <v>0.42424242424242425</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -7179,8 +7277,12 @@
       <c r="H18" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="19" spans="1:8">
+      <c r="I18">
+        <f t="shared" si="0"/>
+        <v>0.42424242424242425</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -7205,8 +7307,12 @@
       <c r="H19" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="20" spans="1:8">
+      <c r="I19">
+        <f t="shared" si="0"/>
+        <v>0.42424242424242425</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -7231,8 +7337,12 @@
       <c r="H20" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="21" spans="1:8">
+      <c r="I20">
+        <f t="shared" si="0"/>
+        <v>0.42424242424242425</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -7257,8 +7367,12 @@
       <c r="H21" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="22" spans="1:8">
+      <c r="I21">
+        <f t="shared" si="0"/>
+        <v>0.42424242424242425</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -7283,8 +7397,12 @@
       <c r="H22" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="23" spans="1:8">
+      <c r="I22">
+        <f t="shared" si="0"/>
+        <v>0.42424242424242425</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23" t="s">
         <v>9</v>
       </c>
@@ -7309,8 +7427,12 @@
       <c r="H23" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="24" spans="1:8">
+      <c r="I23">
+        <f t="shared" si="0"/>
+        <v>0.42424242424242425</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24" t="s">
         <v>9</v>
       </c>
@@ -7335,8 +7457,12 @@
       <c r="H24" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="25" spans="1:8">
+      <c r="I24">
+        <f t="shared" si="0"/>
+        <v>0.42424242424242425</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -7361,8 +7487,12 @@
       <c r="H25" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="26" spans="1:8">
+      <c r="I25">
+        <f t="shared" si="0"/>
+        <v>0.42424242424242425</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26" t="s">
         <v>9</v>
       </c>
@@ -7387,8 +7517,12 @@
       <c r="H26" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="27" spans="1:8">
+      <c r="I26">
+        <f t="shared" si="0"/>
+        <v>0.42424242424242425</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27" t="s">
         <v>9</v>
       </c>
@@ -7413,8 +7547,12 @@
       <c r="H27" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="28" spans="1:8">
+      <c r="I27">
+        <f t="shared" si="0"/>
+        <v>0.42424242424242425</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
       <c r="A28" t="s">
         <v>9</v>
       </c>
@@ -7439,8 +7577,12 @@
       <c r="H28" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="29" spans="1:8">
+      <c r="I28">
+        <f t="shared" si="0"/>
+        <v>0.42424242424242425</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
       <c r="A29" t="s">
         <v>9</v>
       </c>
@@ -7465,8 +7607,12 @@
       <c r="H29" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="30" spans="1:8">
+      <c r="I29">
+        <f t="shared" si="0"/>
+        <v>0.42424242424242425</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
       <c r="A30" t="s">
         <v>9</v>
       </c>
@@ -7491,8 +7637,12 @@
       <c r="H30" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="31" spans="1:8">
+      <c r="I30">
+        <f t="shared" si="0"/>
+        <v>0.42424242424242425</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
       <c r="A31" t="s">
         <v>9</v>
       </c>
@@ -7517,8 +7667,12 @@
       <c r="H31" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="32" spans="1:8">
+      <c r="I31">
+        <f t="shared" si="0"/>
+        <v>0.42424242424242425</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
       <c r="A32" t="s">
         <v>9</v>
       </c>
@@ -7543,8 +7697,12 @@
       <c r="H32" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:8">
+      <c r="I32">
+        <f t="shared" si="0"/>
+        <v>0.42424242424242425</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
       <c r="A33" t="s">
         <v>9</v>
       </c>
@@ -7569,8 +7727,12 @@
       <c r="H33" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="34" spans="1:8">
+      <c r="I33">
+        <f t="shared" si="0"/>
+        <v>0.42424242424242425</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
       <c r="A34" t="s">
         <v>9</v>
       </c>
@@ -7595,8 +7757,12 @@
       <c r="H34" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="35" spans="1:8">
+      <c r="I34">
+        <f t="shared" si="0"/>
+        <v>0.42424242424242425</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
       <c r="A35" t="s">
         <v>63</v>
       </c>
@@ -7621,8 +7787,15 @@
       <c r="H35" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="36" spans="1:8">
+      <c r="I35">
+        <f>22/36</f>
+        <v>0.61111111111111116</v>
+      </c>
+      <c r="J35" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
       <c r="A36" t="s">
         <v>63</v>
       </c>
@@ -7647,8 +7820,12 @@
       <c r="H36" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="37" spans="1:8">
+      <c r="I36">
+        <f>22/36</f>
+        <v>0.61111111111111116</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
       <c r="A37" t="s">
         <v>63</v>
       </c>
@@ -7673,8 +7850,12 @@
       <c r="H37" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="38" spans="1:8">
+      <c r="I37">
+        <f t="shared" ref="I37:I69" si="1">22/36</f>
+        <v>0.61111111111111116</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
       <c r="A38" t="s">
         <v>63</v>
       </c>
@@ -7699,8 +7880,12 @@
       <c r="H38" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="39" spans="1:8">
+      <c r="I38">
+        <f t="shared" si="1"/>
+        <v>0.61111111111111116</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
       <c r="A39" t="s">
         <v>63</v>
       </c>
@@ -7725,8 +7910,12 @@
       <c r="H39" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="40" spans="1:8">
+      <c r="I39">
+        <f t="shared" si="1"/>
+        <v>0.61111111111111116</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
       <c r="A40" t="s">
         <v>63</v>
       </c>
@@ -7751,8 +7940,12 @@
       <c r="H40" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="41" spans="1:8">
+      <c r="I40">
+        <f t="shared" si="1"/>
+        <v>0.61111111111111116</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
       <c r="A41" t="s">
         <v>63</v>
       </c>
@@ -7777,8 +7970,12 @@
       <c r="H41" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="42" spans="1:8">
+      <c r="I41">
+        <f t="shared" si="1"/>
+        <v>0.61111111111111116</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
       <c r="A42" t="s">
         <v>63</v>
       </c>
@@ -7803,8 +8000,12 @@
       <c r="H42" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="43" spans="1:8">
+      <c r="I42">
+        <f t="shared" si="1"/>
+        <v>0.61111111111111116</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
       <c r="A43" t="s">
         <v>63</v>
       </c>
@@ -7829,8 +8030,12 @@
       <c r="H43" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="44" spans="1:8">
+      <c r="I43">
+        <f t="shared" si="1"/>
+        <v>0.61111111111111116</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
       <c r="A44" t="s">
         <v>63</v>
       </c>
@@ -7855,8 +8060,12 @@
       <c r="H44" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="45" spans="1:8">
+      <c r="I44">
+        <f t="shared" si="1"/>
+        <v>0.61111111111111116</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
       <c r="A45" t="s">
         <v>63</v>
       </c>
@@ -7881,8 +8090,12 @@
       <c r="H45" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="46" spans="1:8">
+      <c r="I45">
+        <f t="shared" si="1"/>
+        <v>0.61111111111111116</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
       <c r="A46" t="s">
         <v>63</v>
       </c>
@@ -7907,8 +8120,12 @@
       <c r="H46" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="47" spans="1:8">
+      <c r="I46">
+        <f t="shared" si="1"/>
+        <v>0.61111111111111116</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
       <c r="A47" t="s">
         <v>63</v>
       </c>
@@ -7933,8 +8150,12 @@
       <c r="H47" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="48" spans="1:8">
+      <c r="I47">
+        <f t="shared" si="1"/>
+        <v>0.61111111111111116</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10">
       <c r="A48" t="s">
         <v>63</v>
       </c>
@@ -7959,8 +8180,12 @@
       <c r="H48" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="49" spans="1:8">
+      <c r="I48">
+        <f t="shared" si="1"/>
+        <v>0.61111111111111116</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
       <c r="A49" t="s">
         <v>63</v>
       </c>
@@ -7985,8 +8210,12 @@
       <c r="H49" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="50" spans="1:8">
+      <c r="I49">
+        <f t="shared" si="1"/>
+        <v>0.61111111111111116</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
       <c r="A50" t="s">
         <v>63</v>
       </c>
@@ -8011,8 +8240,12 @@
       <c r="H50" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="51" spans="1:8">
+      <c r="I50">
+        <f t="shared" si="1"/>
+        <v>0.61111111111111116</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
       <c r="A51" t="s">
         <v>63</v>
       </c>
@@ -8037,8 +8270,12 @@
       <c r="H51" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="52" spans="1:8">
+      <c r="I51">
+        <f t="shared" si="1"/>
+        <v>0.61111111111111116</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9">
       <c r="A52" t="s">
         <v>63</v>
       </c>
@@ -8063,8 +8300,12 @@
       <c r="H52" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="53" spans="1:8">
+      <c r="I52">
+        <f t="shared" si="1"/>
+        <v>0.61111111111111116</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9">
       <c r="A53" t="s">
         <v>63</v>
       </c>
@@ -8089,8 +8330,12 @@
       <c r="H53" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="54" spans="1:8">
+      <c r="I53">
+        <f t="shared" si="1"/>
+        <v>0.61111111111111116</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9">
       <c r="A54" t="s">
         <v>63</v>
       </c>
@@ -8115,8 +8360,12 @@
       <c r="H54" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="55" spans="1:8">
+      <c r="I54">
+        <f t="shared" si="1"/>
+        <v>0.61111111111111116</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9">
       <c r="A55" t="s">
         <v>63</v>
       </c>
@@ -8141,8 +8390,12 @@
       <c r="H55" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="56" spans="1:8">
+      <c r="I55">
+        <f t="shared" si="1"/>
+        <v>0.61111111111111116</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9">
       <c r="A56" t="s">
         <v>63</v>
       </c>
@@ -8167,8 +8420,12 @@
       <c r="H56" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="57" spans="1:8">
+      <c r="I56">
+        <f t="shared" si="1"/>
+        <v>0.61111111111111116</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9">
       <c r="A57" t="s">
         <v>63</v>
       </c>
@@ -8193,8 +8450,12 @@
       <c r="H57" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="58" spans="1:8">
+      <c r="I57">
+        <f t="shared" si="1"/>
+        <v>0.61111111111111116</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9">
       <c r="A58" t="s">
         <v>63</v>
       </c>
@@ -8219,8 +8480,12 @@
       <c r="H58" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="59" spans="1:8">
+      <c r="I58">
+        <f t="shared" si="1"/>
+        <v>0.61111111111111116</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9">
       <c r="A59" t="s">
         <v>63</v>
       </c>
@@ -8245,8 +8510,12 @@
       <c r="H59" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="60" spans="1:8">
+      <c r="I59">
+        <f t="shared" si="1"/>
+        <v>0.61111111111111116</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9">
       <c r="A60" t="s">
         <v>63</v>
       </c>
@@ -8271,8 +8540,12 @@
       <c r="H60" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="61" spans="1:8">
+      <c r="I60">
+        <f t="shared" si="1"/>
+        <v>0.61111111111111116</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9">
       <c r="A61" t="s">
         <v>63</v>
       </c>
@@ -8297,8 +8570,12 @@
       <c r="H61" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="62" spans="1:8">
+      <c r="I61">
+        <f t="shared" si="1"/>
+        <v>0.61111111111111116</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9">
       <c r="A62" t="s">
         <v>63</v>
       </c>
@@ -8323,8 +8600,12 @@
       <c r="H62" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="63" spans="1:8">
+      <c r="I62">
+        <f t="shared" si="1"/>
+        <v>0.61111111111111116</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9">
       <c r="A63" t="s">
         <v>63</v>
       </c>
@@ -8349,8 +8630,12 @@
       <c r="H63" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="64" spans="1:8">
+      <c r="I63">
+        <f t="shared" si="1"/>
+        <v>0.61111111111111116</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9">
       <c r="A64" t="s">
         <v>63</v>
       </c>
@@ -8375,8 +8660,12 @@
       <c r="H64" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="65" spans="1:8">
+      <c r="I64">
+        <f t="shared" si="1"/>
+        <v>0.61111111111111116</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10">
       <c r="A65" t="s">
         <v>63</v>
       </c>
@@ -8401,8 +8690,12 @@
       <c r="H65" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="66" spans="1:8">
+      <c r="I65">
+        <f t="shared" si="1"/>
+        <v>0.61111111111111116</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10">
       <c r="A66" t="s">
         <v>63</v>
       </c>
@@ -8427,8 +8720,12 @@
       <c r="H66" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="67" spans="1:8">
+      <c r="I66">
+        <f t="shared" si="1"/>
+        <v>0.61111111111111116</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10">
       <c r="A67" t="s">
         <v>63</v>
       </c>
@@ -8453,8 +8750,12 @@
       <c r="H67" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="68" spans="1:8">
+      <c r="I67">
+        <f t="shared" si="1"/>
+        <v>0.61111111111111116</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10">
       <c r="A68" t="s">
         <v>63</v>
       </c>
@@ -8479,8 +8780,12 @@
       <c r="H68" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="69" spans="1:8">
+      <c r="I68">
+        <f t="shared" si="1"/>
+        <v>0.61111111111111116</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10">
       <c r="A69" t="s">
         <v>63</v>
       </c>
@@ -8505,8 +8810,12 @@
       <c r="H69" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="70" spans="1:8">
+      <c r="I69">
+        <f t="shared" si="1"/>
+        <v>0.61111111111111116</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10">
       <c r="A70" t="s">
         <v>63</v>
       </c>
@@ -8531,8 +8840,12 @@
       <c r="H70" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="71" spans="1:8">
+      <c r="I70">
+        <f>22/36</f>
+        <v>0.61111111111111116</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10">
       <c r="A71" t="s">
         <v>103</v>
       </c>
@@ -8557,8 +8870,15 @@
       <c r="H71" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="72" spans="1:8">
+      <c r="I71">
+        <f>10/33</f>
+        <v>0.30303030303030304</v>
+      </c>
+      <c r="J71" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10">
       <c r="A72" t="s">
         <v>103</v>
       </c>
@@ -8583,8 +8903,12 @@
       <c r="H72" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="73" spans="1:8">
+      <c r="I72">
+        <f>10/33</f>
+        <v>0.30303030303030304</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10">
       <c r="A73" t="s">
         <v>103</v>
       </c>
@@ -8609,8 +8933,12 @@
       <c r="H73" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="74" spans="1:8">
+      <c r="I73">
+        <f t="shared" ref="I73:I103" si="2">10/33</f>
+        <v>0.30303030303030304</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10">
       <c r="A74" t="s">
         <v>103</v>
       </c>
@@ -8635,8 +8963,12 @@
       <c r="H74" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="75" spans="1:8">
+      <c r="I74">
+        <f t="shared" si="2"/>
+        <v>0.30303030303030304</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10">
       <c r="A75" t="s">
         <v>103</v>
       </c>
@@ -8661,8 +8993,12 @@
       <c r="H75" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="76" spans="1:8">
+      <c r="I75">
+        <f t="shared" si="2"/>
+        <v>0.30303030303030304</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10">
       <c r="A76" t="s">
         <v>103</v>
       </c>
@@ -8687,8 +9023,12 @@
       <c r="H76" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="77" spans="1:8">
+      <c r="I76">
+        <f t="shared" si="2"/>
+        <v>0.30303030303030304</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10">
       <c r="A77" t="s">
         <v>103</v>
       </c>
@@ -8713,8 +9053,12 @@
       <c r="H77" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="78" spans="1:8">
+      <c r="I77">
+        <f t="shared" si="2"/>
+        <v>0.30303030303030304</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10">
       <c r="A78" t="s">
         <v>103</v>
       </c>
@@ -8739,8 +9083,12 @@
       <c r="H78" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="79" spans="1:8">
+      <c r="I78">
+        <f t="shared" si="2"/>
+        <v>0.30303030303030304</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10">
       <c r="A79" t="s">
         <v>103</v>
       </c>
@@ -8765,8 +9113,12 @@
       <c r="H79" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="80" spans="1:8">
+      <c r="I79">
+        <f t="shared" si="2"/>
+        <v>0.30303030303030304</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10">
       <c r="A80" t="s">
         <v>103</v>
       </c>
@@ -8791,8 +9143,12 @@
       <c r="H80" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="81" spans="1:8">
+      <c r="I80">
+        <f t="shared" si="2"/>
+        <v>0.30303030303030304</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9">
       <c r="A81" t="s">
         <v>103</v>
       </c>
@@ -8817,8 +9173,12 @@
       <c r="H81" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="82" spans="1:8">
+      <c r="I81">
+        <f t="shared" si="2"/>
+        <v>0.30303030303030304</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9">
       <c r="A82" t="s">
         <v>103</v>
       </c>
@@ -8843,8 +9203,12 @@
       <c r="H82" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="83" spans="1:8">
+      <c r="I82">
+        <f t="shared" si="2"/>
+        <v>0.30303030303030304</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9">
       <c r="A83" t="s">
         <v>103</v>
       </c>
@@ -8869,8 +9233,12 @@
       <c r="H83" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="84" spans="1:8">
+      <c r="I83">
+        <f t="shared" si="2"/>
+        <v>0.30303030303030304</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9">
       <c r="A84" t="s">
         <v>103</v>
       </c>
@@ -8895,8 +9263,12 @@
       <c r="H84" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="85" spans="1:8">
+      <c r="I84">
+        <f t="shared" si="2"/>
+        <v>0.30303030303030304</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9">
       <c r="A85" t="s">
         <v>103</v>
       </c>
@@ -8921,8 +9293,12 @@
       <c r="H85" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="86" spans="1:8">
+      <c r="I85">
+        <f t="shared" si="2"/>
+        <v>0.30303030303030304</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9">
       <c r="A86" t="s">
         <v>103</v>
       </c>
@@ -8947,8 +9323,12 @@
       <c r="H86" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="87" spans="1:8">
+      <c r="I86">
+        <f t="shared" si="2"/>
+        <v>0.30303030303030304</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9">
       <c r="A87" t="s">
         <v>103</v>
       </c>
@@ -8973,8 +9353,12 @@
       <c r="H87" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="88" spans="1:8">
+      <c r="I87">
+        <f t="shared" si="2"/>
+        <v>0.30303030303030304</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9">
       <c r="A88" t="s">
         <v>103</v>
       </c>
@@ -8999,8 +9383,12 @@
       <c r="H88" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="89" spans="1:8">
+      <c r="I88">
+        <f t="shared" si="2"/>
+        <v>0.30303030303030304</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9">
       <c r="A89" t="s">
         <v>103</v>
       </c>
@@ -9025,8 +9413,12 @@
       <c r="H89" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="90" spans="1:8">
+      <c r="I89">
+        <f t="shared" si="2"/>
+        <v>0.30303030303030304</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9">
       <c r="A90" t="s">
         <v>103</v>
       </c>
@@ -9051,8 +9443,12 @@
       <c r="H90" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="91" spans="1:8">
+      <c r="I90">
+        <f t="shared" si="2"/>
+        <v>0.30303030303030304</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9">
       <c r="A91" t="s">
         <v>103</v>
       </c>
@@ -9077,8 +9473,12 @@
       <c r="H91" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="92" spans="1:8">
+      <c r="I91">
+        <f t="shared" si="2"/>
+        <v>0.30303030303030304</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9">
       <c r="A92" t="s">
         <v>103</v>
       </c>
@@ -9103,8 +9503,12 @@
       <c r="H92" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="93" spans="1:8">
+      <c r="I92">
+        <f t="shared" si="2"/>
+        <v>0.30303030303030304</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9">
       <c r="A93" t="s">
         <v>103</v>
       </c>
@@ -9129,8 +9533,12 @@
       <c r="H93" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="94" spans="1:8">
+      <c r="I93">
+        <f t="shared" si="2"/>
+        <v>0.30303030303030304</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9">
       <c r="A94" t="s">
         <v>103</v>
       </c>
@@ -9155,8 +9563,12 @@
       <c r="H94" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="95" spans="1:8">
+      <c r="I94">
+        <f t="shared" si="2"/>
+        <v>0.30303030303030304</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9">
       <c r="A95" t="s">
         <v>103</v>
       </c>
@@ -9181,8 +9593,12 @@
       <c r="H95" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="96" spans="1:8">
+      <c r="I95">
+        <f t="shared" si="2"/>
+        <v>0.30303030303030304</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9">
       <c r="A96" t="s">
         <v>103</v>
       </c>
@@ -9207,8 +9623,12 @@
       <c r="H96" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="97" spans="1:8">
+      <c r="I96">
+        <f t="shared" si="2"/>
+        <v>0.30303030303030304</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9">
       <c r="A97" t="s">
         <v>103</v>
       </c>
@@ -9233,8 +9653,12 @@
       <c r="H97" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="98" spans="1:8">
+      <c r="I97">
+        <f t="shared" si="2"/>
+        <v>0.30303030303030304</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9">
       <c r="A98" t="s">
         <v>103</v>
       </c>
@@ -9259,8 +9683,12 @@
       <c r="H98" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="99" spans="1:8">
+      <c r="I98">
+        <f t="shared" si="2"/>
+        <v>0.30303030303030304</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9">
       <c r="A99" t="s">
         <v>103</v>
       </c>
@@ -9285,8 +9713,12 @@
       <c r="H99" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="100" spans="1:8">
+      <c r="I99">
+        <f t="shared" si="2"/>
+        <v>0.30303030303030304</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9">
       <c r="A100" t="s">
         <v>103</v>
       </c>
@@ -9311,8 +9743,12 @@
       <c r="H100" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="101" spans="1:8">
+      <c r="I100">
+        <f t="shared" si="2"/>
+        <v>0.30303030303030304</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9">
       <c r="A101" t="s">
         <v>103</v>
       </c>
@@ -9337,8 +9773,12 @@
       <c r="H101" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="102" spans="1:8">
+      <c r="I101">
+        <f t="shared" si="2"/>
+        <v>0.30303030303030304</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9">
       <c r="A102" t="s">
         <v>103</v>
       </c>
@@ -9363,8 +9803,12 @@
       <c r="H102" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="103" spans="1:8">
+      <c r="I102">
+        <f t="shared" si="2"/>
+        <v>0.30303030303030304</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9">
       <c r="A103" t="s">
         <v>103</v>
       </c>
@@ -9389,8 +9833,12 @@
       <c r="H103" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="104" spans="1:8">
+      <c r="I103">
+        <f t="shared" si="2"/>
+        <v>0.30303030303030304</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9">
       <c r="A104" t="s">
         <v>141</v>
       </c>
@@ -9415,8 +9863,12 @@
       <c r="H104" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="105" spans="1:8">
+      <c r="I104">
+        <f>2/10</f>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9">
       <c r="A105" t="s">
         <v>141</v>
       </c>
@@ -9441,8 +9893,12 @@
       <c r="H105" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="106" spans="1:8">
+      <c r="I105">
+        <f>2/10</f>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9">
       <c r="A106" t="s">
         <v>141</v>
       </c>
@@ -9467,8 +9923,12 @@
       <c r="H106" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="107" spans="1:8">
+      <c r="I106">
+        <f t="shared" ref="I106:I123" si="3">2/10</f>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9">
       <c r="A107" t="s">
         <v>141</v>
       </c>
@@ -9493,8 +9953,12 @@
       <c r="H107" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="108" spans="1:8">
+      <c r="I107">
+        <f t="shared" si="3"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9">
       <c r="A108" t="s">
         <v>141</v>
       </c>
@@ -9519,8 +9983,12 @@
       <c r="H108" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="109" spans="1:8">
+      <c r="I108">
+        <f t="shared" si="3"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9">
       <c r="A109" t="s">
         <v>141</v>
       </c>
@@ -9545,8 +10013,12 @@
       <c r="H109" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="110" spans="1:8">
+      <c r="I109">
+        <f t="shared" si="3"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9">
       <c r="A110" t="s">
         <v>141</v>
       </c>
@@ -9571,8 +10043,12 @@
       <c r="H110" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="111" spans="1:8">
+      <c r="I110">
+        <f t="shared" si="3"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9">
       <c r="A111" t="s">
         <v>141</v>
       </c>
@@ -9597,8 +10073,12 @@
       <c r="H111" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="112" spans="1:8">
+      <c r="I111">
+        <f t="shared" si="3"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9">
       <c r="A112" t="s">
         <v>141</v>
       </c>
@@ -9623,8 +10103,12 @@
       <c r="H112" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="113" spans="1:8">
+      <c r="I112">
+        <f t="shared" si="3"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9">
       <c r="A113" t="s">
         <v>141</v>
       </c>
@@ -9649,8 +10133,12 @@
       <c r="H113" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="114" spans="1:8">
+      <c r="I113">
+        <f t="shared" si="3"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9">
       <c r="A114" t="s">
         <v>160</v>
       </c>
@@ -9675,8 +10163,12 @@
       <c r="H114" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="115" spans="1:8">
+      <c r="I114">
+        <f>2/10</f>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9">
       <c r="A115" t="s">
         <v>160</v>
       </c>
@@ -9701,8 +10193,12 @@
       <c r="H115" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="116" spans="1:8">
+      <c r="I115">
+        <f t="shared" si="3"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9">
       <c r="A116" t="s">
         <v>160</v>
       </c>
@@ -9727,8 +10223,12 @@
       <c r="H116" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="117" spans="1:8">
+      <c r="I116">
+        <f t="shared" si="3"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9">
       <c r="A117" t="s">
         <v>160</v>
       </c>
@@ -9753,8 +10253,12 @@
       <c r="H117" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="118" spans="1:8">
+      <c r="I117">
+        <f t="shared" si="3"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9">
       <c r="A118" t="s">
         <v>160</v>
       </c>
@@ -9779,8 +10283,12 @@
       <c r="H118" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="119" spans="1:8">
+      <c r="I118">
+        <f t="shared" si="3"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9">
       <c r="A119" t="s">
         <v>160</v>
       </c>
@@ -9805,8 +10313,12 @@
       <c r="H119" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="120" spans="1:8">
+      <c r="I119">
+        <f t="shared" si="3"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9">
       <c r="A120" t="s">
         <v>160</v>
       </c>
@@ -9831,8 +10343,12 @@
       <c r="H120" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="121" spans="1:8">
+      <c r="I120">
+        <f t="shared" si="3"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9">
       <c r="A121" t="s">
         <v>160</v>
       </c>
@@ -9857,8 +10373,12 @@
       <c r="H121" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="122" spans="1:8">
+      <c r="I121">
+        <f t="shared" si="3"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9">
       <c r="A122" t="s">
         <v>160</v>
       </c>
@@ -9883,8 +10403,12 @@
       <c r="H122" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="123" spans="1:8">
+      <c r="I122">
+        <f t="shared" si="3"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9">
       <c r="A123" t="s">
         <v>160</v>
       </c>
@@ -9909,8 +10433,12 @@
       <c r="H123" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="124" spans="1:8">
+      <c r="I123">
+        <f t="shared" si="3"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9">
       <c r="A124" t="s">
         <v>172</v>
       </c>
@@ -9935,8 +10463,11 @@
       <c r="H124" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="125" spans="1:8">
+      <c r="I124">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9">
       <c r="A125" t="s">
         <v>172</v>
       </c>
@@ -9961,8 +10492,11 @@
       <c r="H125" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="126" spans="1:8">
+      <c r="I125">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9">
       <c r="A126" t="s">
         <v>172</v>
       </c>
@@ -9987,8 +10521,11 @@
       <c r="H126" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="127" spans="1:8">
+      <c r="I126">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9">
       <c r="A127" t="s">
         <v>172</v>
       </c>
@@ -10013,8 +10550,11 @@
       <c r="H127" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="128" spans="1:8">
+      <c r="I127">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9">
       <c r="A128" t="s">
         <v>172</v>
       </c>
@@ -10039,8 +10579,11 @@
       <c r="H128" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="129" spans="1:8">
+      <c r="I128">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9">
       <c r="A129" t="s">
         <v>172</v>
       </c>
@@ -10065,8 +10608,11 @@
       <c r="H129" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="130" spans="1:8">
+      <c r="I129">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9">
       <c r="A130" t="s">
         <v>172</v>
       </c>
@@ -10091,8 +10637,11 @@
       <c r="H130" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="131" spans="1:8">
+      <c r="I130">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9">
       <c r="A131" t="s">
         <v>172</v>
       </c>
@@ -10117,8 +10666,11 @@
       <c r="H131" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="132" spans="1:8">
+      <c r="I131">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9">
       <c r="A132" t="s">
         <v>172</v>
       </c>
@@ -10143,8 +10695,11 @@
       <c r="H132" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="133" spans="1:8">
+      <c r="I132">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9">
       <c r="A133" t="s">
         <v>172</v>
       </c>
@@ -10169,8 +10724,11 @@
       <c r="H133" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="134" spans="1:8">
+      <c r="I133">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9">
       <c r="A134" t="s">
         <v>183</v>
       </c>
@@ -10195,8 +10753,12 @@
       <c r="H134" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="135" spans="1:8">
+      <c r="I134">
+        <f>1/10</f>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9">
       <c r="A135" t="s">
         <v>183</v>
       </c>
@@ -10221,8 +10783,11 @@
       <c r="H135" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="136" spans="1:8">
+      <c r="I135">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9">
       <c r="A136" t="s">
         <v>183</v>
       </c>
@@ -10247,8 +10812,11 @@
       <c r="H136" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="137" spans="1:8">
+      <c r="I136">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9">
       <c r="A137" t="s">
         <v>183</v>
       </c>
@@ -10273,8 +10841,12 @@
       <c r="H137" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="138" spans="1:8">
+      <c r="I137">
+        <f t="shared" ref="I137:I143" si="4">1/10</f>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9">
       <c r="A138" t="s">
         <v>183</v>
       </c>
@@ -10299,8 +10871,11 @@
       <c r="H138" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="139" spans="1:8">
+      <c r="I138">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9">
       <c r="A139" t="s">
         <v>183</v>
       </c>
@@ -10325,8 +10900,11 @@
       <c r="H139" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="140" spans="1:8">
+      <c r="I139">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9">
       <c r="A140" t="s">
         <v>183</v>
       </c>
@@ -10351,8 +10929,12 @@
       <c r="H140" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="141" spans="1:8">
+      <c r="I140">
+        <f t="shared" ref="I140:I143" si="5">1/10</f>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9">
       <c r="A141" t="s">
         <v>183</v>
       </c>
@@ -10377,8 +10959,11 @@
       <c r="H141" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="142" spans="1:8">
+      <c r="I141">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9">
       <c r="A142" t="s">
         <v>183</v>
       </c>
@@ -10403,8 +10988,11 @@
       <c r="H142" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="143" spans="1:8">
+      <c r="I142">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9">
       <c r="A143" t="s">
         <v>183</v>
       </c>
@@ -10429,8 +11017,12 @@
       <c r="H143" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="144" spans="1:8">
+      <c r="I143">
+        <f t="shared" ref="I143" si="6">1/10</f>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9">
       <c r="A144" t="s">
         <v>194</v>
       </c>
@@ -10455,8 +11047,11 @@
       <c r="H144" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="145" spans="1:8">
+      <c r="I144">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9">
       <c r="A145" t="s">
         <v>194</v>
       </c>
@@ -10481,8 +11076,11 @@
       <c r="H145" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="146" spans="1:8">
+      <c r="I145">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9">
       <c r="A146" t="s">
         <v>194</v>
       </c>
@@ -10507,8 +11105,11 @@
       <c r="H146" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="147" spans="1:8">
+      <c r="I146">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9">
       <c r="A147" t="s">
         <v>194</v>
       </c>
@@ -10533,8 +11134,11 @@
       <c r="H147" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="148" spans="1:8">
+      <c r="I147">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9">
       <c r="A148" t="s">
         <v>194</v>
       </c>
@@ -10559,8 +11163,11 @@
       <c r="H148" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="149" spans="1:8">
+      <c r="I148">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9">
       <c r="A149" t="s">
         <v>194</v>
       </c>
@@ -10585,8 +11192,11 @@
       <c r="H149" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="150" spans="1:8">
+      <c r="I149">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="150" spans="1:9">
       <c r="A150" t="s">
         <v>194</v>
       </c>
@@ -10611,8 +11221,11 @@
       <c r="H150" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="151" spans="1:8">
+      <c r="I150">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="151" spans="1:9">
       <c r="A151" t="s">
         <v>194</v>
       </c>
@@ -10637,8 +11250,11 @@
       <c r="H151" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="152" spans="1:8">
+      <c r="I151">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9">
       <c r="A152" t="s">
         <v>194</v>
       </c>
@@ -10663,8 +11279,11 @@
       <c r="H152" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="153" spans="1:8">
+      <c r="I152">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="153" spans="1:9">
       <c r="A153" t="s">
         <v>194</v>
       </c>
@@ -10689,8 +11308,11 @@
       <c r="H153" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="154" spans="1:8">
+      <c r="I153">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9">
       <c r="A154" t="s">
         <v>205</v>
       </c>
@@ -10715,8 +11337,11 @@
       <c r="H154" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="155" spans="1:8">
+      <c r="I154">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="155" spans="1:9">
       <c r="A155" t="s">
         <v>205</v>
       </c>
@@ -10741,8 +11366,11 @@
       <c r="H155" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="156" spans="1:8">
+      <c r="I155">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="156" spans="1:9">
       <c r="A156" t="s">
         <v>205</v>
       </c>
@@ -10767,8 +11395,11 @@
       <c r="H156" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="157" spans="1:8">
+      <c r="I156">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9">
       <c r="A157" t="s">
         <v>205</v>
       </c>
@@ -10793,8 +11424,11 @@
       <c r="H157" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="158" spans="1:8">
+      <c r="I157">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="158" spans="1:9">
       <c r="A158" t="s">
         <v>205</v>
       </c>
@@ -10819,8 +11453,11 @@
       <c r="H158" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="159" spans="1:8">
+      <c r="I158">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9">
       <c r="A159" t="s">
         <v>205</v>
       </c>
@@ -10845,8 +11482,11 @@
       <c r="H159" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="160" spans="1:8">
+      <c r="I159">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9">
       <c r="A160" t="s">
         <v>205</v>
       </c>
@@ -10871,8 +11511,11 @@
       <c r="H160" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="161" spans="1:8">
+      <c r="I160">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9">
       <c r="A161" t="s">
         <v>205</v>
       </c>
@@ -10897,8 +11540,11 @@
       <c r="H161" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="162" spans="1:8">
+      <c r="I161">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="162" spans="1:9">
       <c r="A162" t="s">
         <v>205</v>
       </c>
@@ -10923,8 +11569,11 @@
       <c r="H162" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="163" spans="1:8">
+      <c r="I162">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="163" spans="1:9">
       <c r="A163" t="s">
         <v>205</v>
       </c>
@@ -10949,8 +11598,11 @@
       <c r="H163" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="164" spans="1:8">
+      <c r="I163">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9">
       <c r="A164" t="s">
         <v>217</v>
       </c>
@@ -10975,8 +11627,11 @@
       <c r="H164" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="165" spans="1:8">
+      <c r="I164">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9">
       <c r="A165" t="s">
         <v>217</v>
       </c>
@@ -11001,8 +11656,11 @@
       <c r="H165" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="166" spans="1:8">
+      <c r="I165">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:9">
       <c r="A166" t="s">
         <v>217</v>
       </c>
@@ -11027,8 +11685,11 @@
       <c r="H166" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="167" spans="1:8">
+      <c r="I166">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="1:9">
       <c r="A167" t="s">
         <v>217</v>
       </c>
@@ -11053,8 +11714,11 @@
       <c r="H167" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="168" spans="1:8">
+      <c r="I167">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:9">
       <c r="A168" t="s">
         <v>217</v>
       </c>
@@ -11079,8 +11743,11 @@
       <c r="H168" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="169" spans="1:8">
+      <c r="I168">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:9">
       <c r="A169" t="s">
         <v>217</v>
       </c>
@@ -11105,8 +11772,11 @@
       <c r="H169" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="170" spans="1:8">
+      <c r="I169">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="1:9">
       <c r="A170" t="s">
         <v>217</v>
       </c>
@@ -11131,8 +11801,11 @@
       <c r="H170" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="171" spans="1:8">
+      <c r="I170">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:9">
       <c r="A171" t="s">
         <v>217</v>
       </c>
@@ -11157,8 +11830,11 @@
       <c r="H171" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="172" spans="1:8">
+      <c r="I171">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:9">
       <c r="A172" t="s">
         <v>217</v>
       </c>
@@ -11183,8 +11859,11 @@
       <c r="H172" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="173" spans="1:8">
+      <c r="I172">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:9">
       <c r="A173" t="s">
         <v>217</v>
       </c>
@@ -11209,8 +11888,11 @@
       <c r="H173" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="174" spans="1:8">
+      <c r="I173">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="1:9">
       <c r="A174" t="s">
         <v>231</v>
       </c>
@@ -11235,8 +11917,11 @@
       <c r="H174" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="175" spans="1:8">
+      <c r="I174">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="175" spans="1:9">
       <c r="A175" t="s">
         <v>231</v>
       </c>
@@ -11261,8 +11946,11 @@
       <c r="H175" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="176" spans="1:8">
+      <c r="I175">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="176" spans="1:9">
       <c r="A176" t="s">
         <v>231</v>
       </c>
@@ -11287,8 +11975,11 @@
       <c r="H176" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="177" spans="1:8">
+      <c r="I176">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="177" spans="1:9">
       <c r="A177" t="s">
         <v>231</v>
       </c>
@@ -11313,8 +12004,11 @@
       <c r="H177" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="178" spans="1:8">
+      <c r="I177">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="178" spans="1:9">
       <c r="A178" t="s">
         <v>231</v>
       </c>
@@ -11339,8 +12033,11 @@
       <c r="H178" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="179" spans="1:8">
+      <c r="I178">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="179" spans="1:9">
       <c r="A179" t="s">
         <v>231</v>
       </c>
@@ -11365,8 +12062,11 @@
       <c r="H179" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="180" spans="1:8">
+      <c r="I179">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="180" spans="1:9">
       <c r="A180" t="s">
         <v>231</v>
       </c>
@@ -11391,8 +12091,11 @@
       <c r="H180" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="181" spans="1:8">
+      <c r="I180">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="181" spans="1:9">
       <c r="A181" t="s">
         <v>231</v>
       </c>
@@ -11417,8 +12120,11 @@
       <c r="H181" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="182" spans="1:8">
+      <c r="I181">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="182" spans="1:9">
       <c r="A182" t="s">
         <v>231</v>
       </c>
@@ -11443,8 +12149,11 @@
       <c r="H182" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="183" spans="1:8">
+      <c r="I182">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="183" spans="1:9">
       <c r="A183" t="s">
         <v>231</v>
       </c>
@@ -11469,8 +12178,11 @@
       <c r="H183" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="184" spans="1:8">
+      <c r="I183">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="184" spans="1:9">
       <c r="A184" t="s">
         <v>244</v>
       </c>
@@ -11495,8 +12207,11 @@
       <c r="H184" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="185" spans="1:8">
+      <c r="I184">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="1:9">
       <c r="A185" t="s">
         <v>244</v>
       </c>
@@ -11521,8 +12236,11 @@
       <c r="H185" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="186" spans="1:8">
+      <c r="I185">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" spans="1:9">
       <c r="A186" t="s">
         <v>244</v>
       </c>
@@ -11547,8 +12265,11 @@
       <c r="H186" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="187" spans="1:8">
+      <c r="I186">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" spans="1:9">
       <c r="A187" t="s">
         <v>244</v>
       </c>
@@ -11573,8 +12294,11 @@
       <c r="H187" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="188" spans="1:8">
+      <c r="I187">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188" spans="1:9">
       <c r="A188" t="s">
         <v>244</v>
       </c>
@@ -11599,8 +12323,11 @@
       <c r="H188" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="189" spans="1:8">
+      <c r="I188">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="189" spans="1:9">
       <c r="A189" t="s">
         <v>244</v>
       </c>
@@ -11625,8 +12352,11 @@
       <c r="H189" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="190" spans="1:8">
+      <c r="I189">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" spans="1:9">
       <c r="A190" t="s">
         <v>244</v>
       </c>
@@ -11651,8 +12381,11 @@
       <c r="H190" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="191" spans="1:8">
+      <c r="I190">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="1:9">
       <c r="A191" t="s">
         <v>244</v>
       </c>
@@ -11677,8 +12410,11 @@
       <c r="H191" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="192" spans="1:8">
+      <c r="I191">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="1:9">
       <c r="A192" t="s">
         <v>244</v>
       </c>
@@ -11703,8 +12439,11 @@
       <c r="H192" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="193" spans="1:8">
+      <c r="I192">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" spans="1:9">
       <c r="A193" t="s">
         <v>244</v>
       </c>
@@ -11729,9 +12468,13 @@
       <c r="H193" t="s">
         <v>31</v>
       </c>
+      <c r="I193">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
more edits - need to figure out problems with which cobbles should be included in the analysis for E2 and possibly E3
</commit_message>
<xml_diff>
--- a/During experiment recording_fixed02.11.2014.xlsx
+++ b/During experiment recording_fixed02.11.2014.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
-  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="1920" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Bipolar" sheetId="1" r:id="rId1"/>
     <sheet name="Free Hand" sheetId="2" r:id="rId2"/>
-    <sheet name="R input" sheetId="3" r:id="rId3"/>
+    <sheet name="During experiment recording_fix" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2423" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2422" uniqueCount="260">
   <si>
     <t>Participant number</t>
   </si>
@@ -6725,8 +6725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A165" workbookViewId="0">
-      <selection activeCell="K192" sqref="K192"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G136" sqref="G136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -10127,8 +10127,8 @@
       <c r="F113" t="s">
         <v>31</v>
       </c>
-      <c r="G113" t="s">
-        <v>140</v>
+      <c r="G113">
+        <v>200</v>
       </c>
       <c r="H113" t="s">
         <v>31</v>
@@ -10742,13 +10742,13 @@
         <v>155</v>
       </c>
       <c r="E134" s="3">
-        <v>155.78</v>
+        <v>115.78</v>
       </c>
       <c r="F134" t="s">
         <v>31</v>
       </c>
       <c r="G134">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="H134" t="s">
         <v>31</v>
@@ -10778,7 +10778,7 @@
         <v>31</v>
       </c>
       <c r="G135">
-        <v>59</v>
+        <v>281</v>
       </c>
       <c r="H135" t="s">
         <v>31</v>
@@ -10807,7 +10807,7 @@
         <v>31</v>
       </c>
       <c r="G136">
-        <v>281</v>
+        <v>299</v>
       </c>
       <c r="H136" t="s">
         <v>31</v>
@@ -10830,19 +10830,19 @@
         <v>12</v>
       </c>
       <c r="E137" s="3">
-        <v>136.36000000000001</v>
+        <v>76.36</v>
       </c>
       <c r="F137" t="s">
         <v>31</v>
       </c>
       <c r="G137">
-        <v>299</v>
+        <v>106</v>
       </c>
       <c r="H137" t="s">
         <v>31</v>
       </c>
       <c r="I137">
-        <f t="shared" ref="I137:I143" si="4">1/10</f>
+        <f t="shared" ref="I137" si="4">1/10</f>
         <v>0.1</v>
       </c>
     </row>
@@ -10860,13 +10860,13 @@
         <v>12</v>
       </c>
       <c r="E138" s="3">
-        <v>176.47</v>
+        <v>116.47</v>
       </c>
       <c r="F138" t="s">
         <v>31</v>
       </c>
       <c r="G138">
-        <v>106</v>
+        <v>138</v>
       </c>
       <c r="H138" t="s">
         <v>31</v>
@@ -10895,7 +10895,7 @@
         <v>31</v>
       </c>
       <c r="G139">
-        <v>138</v>
+        <v>4</v>
       </c>
       <c r="H139" t="s">
         <v>13</v>
@@ -10924,13 +10924,13 @@
         <v>31</v>
       </c>
       <c r="G140">
-        <v>4</v>
+        <v>262</v>
       </c>
       <c r="H140" t="s">
         <v>31</v>
       </c>
       <c r="I140">
-        <f t="shared" ref="I140:I143" si="5">1/10</f>
+        <f t="shared" ref="I140" si="5">1/10</f>
         <v>0.1</v>
       </c>
     </row>
@@ -10954,7 +10954,7 @@
         <v>31</v>
       </c>
       <c r="G141">
-        <v>262</v>
+        <v>320</v>
       </c>
       <c r="H141" t="s">
         <v>31</v>
@@ -10983,7 +10983,7 @@
         <v>31</v>
       </c>
       <c r="G142">
-        <v>320</v>
+        <v>197</v>
       </c>
       <c r="H142" t="s">
         <v>31</v>
@@ -11012,7 +11012,7 @@
         <v>31</v>
       </c>
       <c r="G143">
-        <v>197</v>
+        <v>292</v>
       </c>
       <c r="H143" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
new tables and plots after adding avg time and strikes for N2 'retired' cobbles
</commit_message>
<xml_diff>
--- a/During experiment recording_fixed02.11.2014.xlsx
+++ b/During experiment recording_fixed02.11.2014.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2422" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2420" uniqueCount="262">
   <si>
     <t>Participant number</t>
   </si>
@@ -801,6 +801,12 @@
   </si>
   <si>
     <t>divided by 36</t>
+  </si>
+  <si>
+    <t>N2 avg time</t>
+  </si>
+  <si>
+    <t>N2 avg strikes</t>
   </si>
 </sst>
 </file>
@@ -813,6 +819,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -864,8 +871,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="61">
+  <cellStyleXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -934,7 +947,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="61">
+  <cellStyles count="67">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -965,6 +978,9 @@
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -995,6 +1011,9 @@
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6735,10 +6754,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J193"/>
+  <dimension ref="A1:M207"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54:XFD55"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="G198" sqref="G198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -12381,14 +12400,14 @@
       <c r="D190" t="s">
         <v>255</v>
       </c>
-      <c r="E190" s="3" t="s">
-        <v>61</v>
+      <c r="E190" s="3">
+        <v>97.93</v>
       </c>
       <c r="F190" t="s">
         <v>61</v>
       </c>
-      <c r="G190" t="s">
-        <v>61</v>
+      <c r="G190">
+        <v>133</v>
       </c>
       <c r="H190" t="s">
         <v>31</v>
@@ -12410,14 +12429,14 @@
       <c r="D191" t="s">
         <v>255</v>
       </c>
-      <c r="E191" s="3" t="s">
-        <v>61</v>
+      <c r="E191" s="3">
+        <v>97.93</v>
       </c>
       <c r="F191" t="s">
         <v>61</v>
       </c>
-      <c r="G191" t="s">
-        <v>61</v>
+      <c r="G191">
+        <v>133</v>
       </c>
       <c r="H191" t="s">
         <v>31</v>
@@ -12455,7 +12474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:9">
+    <row r="193" spans="1:13">
       <c r="A193" t="s">
         <v>244</v>
       </c>
@@ -12482,6 +12501,88 @@
       </c>
       <c r="I193">
         <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="1:13">
+      <c r="L197" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="M197" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="198" spans="1:13">
+      <c r="L198" s="3">
+        <v>151.91999999999999</v>
+      </c>
+      <c r="M198">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="199" spans="1:13">
+      <c r="L199" s="3">
+        <v>10.08</v>
+      </c>
+      <c r="M199">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="200" spans="1:13">
+      <c r="L200" s="3">
+        <v>167.08</v>
+      </c>
+      <c r="M200">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="201" spans="1:13">
+      <c r="L201" s="3">
+        <v>145.62</v>
+      </c>
+      <c r="M201">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="202" spans="1:13">
+      <c r="L202" s="3">
+        <v>134.38</v>
+      </c>
+      <c r="M202">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="203" spans="1:13">
+      <c r="L203" s="3">
+        <v>87.5</v>
+      </c>
+      <c r="M203">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="204" spans="1:13">
+      <c r="L204" s="3">
+        <v>52.08</v>
+      </c>
+      <c r="M204">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="205" spans="1:13">
+      <c r="L205" s="3">
+        <v>34.78</v>
+      </c>
+      <c r="M205">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="207" spans="1:13">
+      <c r="L207" s="3">
+        <f>AVERAGE(L198:L205)</f>
+        <v>97.93</v>
+      </c>
+      <c r="M207">
+        <f>AVERAGE(M198:M205)</f>
+        <v>132.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>